<commit_message>
se agrega el codigo VHDL del banco de registros de la consigna 3
</commit_message>
<xml_diff>
--- a/diseño logico tp 1.xlsx
+++ b/diseño logico tp 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan\Desktop\Diseño Logico TP 2024C2\tp-diseno-logico-untref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B4437BA-8BF1-448E-BED4-32AAFF8B8507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25112A4-D58F-4357-9F6E-289E1D4BB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{CD42A113-4D51-4E6E-A94A-7A8F321F0B64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD42A113-4D51-4E6E-A94A-7A8F321F0B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -206,8 +206,12 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,272 +548,273 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C096664D-3F77-4F58-BA1D-A377FEE19EBD}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>